<commit_message>
added shift dropdown in excel, resolved bugs - Bug 562, 571, 567
</commit_message>
<xml_diff>
--- a/AttendanceManagement/wwwroot/ExcelTemplates/Assign Shift.xlsx
+++ b/AttendanceManagement/wwwroot/ExcelTemplates/Assign Shift.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E49164A5-8B0A-43ED-ABE3-9D88131688EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\internship041\source\repos\VLead Attendance Management System\Vlead\AttendanceManagement\wwwroot\ExcelTemplates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E9E60B-CA96-424C-8B09-5EA5AAEDA980}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -20,10 +26,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -40,6 +46,60 @@
   </si>
   <si>
     <t>ShiftName</t>
+  </si>
+  <si>
+    <t>Morning Shift(07:00-15:30)</t>
+  </si>
+  <si>
+    <t>Early Shift(06:00-14:30)</t>
+  </si>
+  <si>
+    <t>Saturday Shift(06:00-11:00)</t>
+  </si>
+  <si>
+    <t>General Shift(08:00-16:30)</t>
+  </si>
+  <si>
+    <t>Sat Shift(08:00-13:00)</t>
+  </si>
+  <si>
+    <t>Day Shift(09:00-17:30)</t>
+  </si>
+  <si>
+    <t>Extended Day Shift(10:00-18:30)</t>
+  </si>
+  <si>
+    <t>Mid Shift(12:00-20:30)</t>
+  </si>
+  <si>
+    <t>Afternoon Shift(14:00-22:30)</t>
+  </si>
+  <si>
+    <t>Evening Shift(15:00-00:00)</t>
+  </si>
+  <si>
+    <t>Late Evening Shift(16:00-01:00)</t>
+  </si>
+  <si>
+    <t>Late Shift(17:00-02:00)</t>
+  </si>
+  <si>
+    <t>Night Shift(18:00-03:00)</t>
+  </si>
+  <si>
+    <t>Extended Night Shift(18:30-03:30)</t>
+  </si>
+  <si>
+    <t>Late Night Shift(19:30-04:30)</t>
+  </si>
+  <si>
+    <t>Overnight Shift(21:00-06:00)</t>
+  </si>
+  <si>
+    <t>Midnight Shift(22:00-07:00)</t>
+  </si>
+  <si>
+    <t>Weekly Off(00:00-00:00)</t>
   </si>
 </sst>
 </file>
@@ -75,8 +135,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,13 +472,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -430,6 +495,129 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F5FF0B10-0730-4062-AE89-6C7E570B8E1C}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$1:$A$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBA5230-B47C-4066-8758-0C24ACBB8A18}">
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="30.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated code in assign shift excel implemented shift dropdown and added role id in search endpoint
</commit_message>
<xml_diff>
--- a/AttendanceManagement/wwwroot/ExcelTemplates/Assign Shift.xlsx
+++ b/AttendanceManagement/wwwroot/ExcelTemplates/Assign Shift.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29227"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E49164A5-8B0A-43ED-ABE3-9D88131688EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{463D5813-1B30-4034-BA42-A0A15FD56320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -40,6 +41,60 @@
   </si>
   <si>
     <t>ShiftName</t>
+  </si>
+  <si>
+    <t>Early Shift(06:00-14:30)</t>
+  </si>
+  <si>
+    <t>Saturday Shift(06:00-11:00)</t>
+  </si>
+  <si>
+    <t>Morning Shift(07:00-15:30)</t>
+  </si>
+  <si>
+    <t>General Shift(08:00-16:30)</t>
+  </si>
+  <si>
+    <t>Sat Shift(08:00-13:00)</t>
+  </si>
+  <si>
+    <t>Day Shift(09:00-17:30)</t>
+  </si>
+  <si>
+    <t>Extended Day Shift(10:00-18:30)</t>
+  </si>
+  <si>
+    <t>Mid Shift(12:00-20:30)</t>
+  </si>
+  <si>
+    <t>Afternoon Shift(14:00-22:30)</t>
+  </si>
+  <si>
+    <t>Evening Shift(15:00-00:00)</t>
+  </si>
+  <si>
+    <t>Late Evening Shift(16:00-01:00)</t>
+  </si>
+  <si>
+    <t>Late Shift(17:00-02:00)</t>
+  </si>
+  <si>
+    <t>Night Shift(18:00-03:00)</t>
+  </si>
+  <si>
+    <t>Extended Night Shift(18:30-03:30)</t>
+  </si>
+  <si>
+    <t>Late Night Shift(19:30-04:30)</t>
+  </si>
+  <si>
+    <t>Overnight Shift(21:00-06:00)</t>
+  </si>
+  <si>
+    <t>Midnight Shift(22:00-07:00)</t>
+  </si>
+  <si>
+    <t>Weekly Off(00:00-00:00)</t>
   </si>
 </sst>
 </file>
@@ -414,7 +469,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -432,5 +487,125 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F5FF0B10-0730-4062-AE89-6C7E570B8E1C}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$1:$A$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBA5230-B47C-4066-8758-0C24ACBB8A18}">
+  <dimension ref="A1:A18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>